<commit_message>
added ny to scraper capability
</commit_message>
<xml_diff>
--- a/src/protest_data.xlsx
+++ b/src/protest_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,6 +685,190 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>March to Protect The Results!</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10019, United States</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>10019</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SAT, NOV 7, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Tell Melinda Katz: COVID Behind Bars = Death</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>125-01 Queens Blvd, Kew Gardens, NY 11415, United States</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>11415</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>MON, JUL 13, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Pre-Super Tuesday #NeverBloomberg March</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1216 5th Ave. New York, NY 10029 (at E. 103 St.)</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>10029</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>SAT, FEB 29, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Make Billionaires Pay Town Hall</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>470 Vanderbilt Ave, Brooklyn, NY 11238-2208, United States</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>11238</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>THU, FEB 27, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Movement for a Green New Deal Town Hall</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>713 Caton Ave, Brooklyn, NY 11218-2661, United States</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>11218</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>THU, FEB 20, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Make Billionaires Pay! Community Town Hall</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>61 Broadway, Ny, Ny 10006</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>10006</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SAT, FEB 8, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Mental Health Care and the New York Health Act: A Panel Discussion</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>131 West 33rd Street, New York, NY 10001</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>10001</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>THU, JAN 30, 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Arena NYC Monthly Meetup with Ritchie Torres</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>171 Elizabeth St, New York, NY 10012-4607, United States</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>10012</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>MON, JAN 27, 2020</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>